<commit_message>
fixing bugs with multiple unrelated numbers
</commit_message>
<xml_diff>
--- a/DAL/conversions.xlsx
+++ b/DAL/conversions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Fun projects\RecipeConverter\RecipeConvertor\DAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Fun projects\RecipeConverter2\DAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55E3030E-1FF3-46AE-9AA2-B35C66351526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AB8D56-B1E4-45A7-9DE0-3B775CA842CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="conversions" sheetId="1" r:id="rId1"/>
@@ -162,8 +162,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,343 +449,340 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A26:D54"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="14.09765625" customWidth="1"/>
-    <col min="6" max="6" width="15.3984375" customWidth="1"/>
-    <col min="7" max="7" width="14.59765625" customWidth="1"/>
-    <col min="9" max="9" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="16384" width="14.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>227</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>14.2</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
         <v>4.7300000000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>198</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>198</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <v>12.5</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="1">
         <v>4.2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>113</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>156</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <v>142</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="1">
         <v>20</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="1">
         <v>12</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="1">
         <v>17.059999999999999</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <v>208</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
         <v>13</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="1">
         <v>4.2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>240</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="1">
         <v>125</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1">
         <v>216</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="1">
         <v>14</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1">
         <v>230</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1">
         <v>198</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="1">
         <v>14.15</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="1">
         <v>4.5</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="1">
         <v>237</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="1">
         <v>15</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="1">
         <v>4.93</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="1">
         <v>3.11</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="1">
         <v>85</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="1">
         <v>5.5</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="1">
         <v>2.46</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="1">
         <v>138</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="1">
         <v>6.8</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="1">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="1">
         <v>8.4</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="1">
         <v>2.8</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="1">
         <v>7</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="1">
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="1">
         <v>6.9</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="1">
         <v>2.4</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="1">
         <v>3.3</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="1">
         <v>1.2</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="1">
         <v>5.6</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="1">
         <v>1.7</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="1">
         <v>239</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="1">
         <v>14.9</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="1">
         <v>255</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="1">
         <v>16</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="1">
         <v>5.3</v>
       </c>
     </row>

</xml_diff>